<commit_message>
sand pool 30 percent commit
</commit_message>
<xml_diff>
--- a/ONSData6DistrictLevel.xlsx
+++ b/ONSData6DistrictLevel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fintech Sandpit\ESG-entity-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43CB272-0661-42D1-8119-24F7292471CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EA200E-E40D-4A4F-9291-6114A3D63550}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{692A125E-7669-4FF7-9E0A-E17AE87AD601}"/>
   </bookViews>
@@ -2405,22 +2405,22 @@
     <t>Folkestone and Hythe</t>
   </si>
   <si>
-    <t>45-45 : Motor trades</t>
-  </si>
-  <si>
-    <t>47-47 : Retail</t>
-  </si>
-  <si>
-    <t>46-46 : Wholesale</t>
-  </si>
-  <si>
-    <t>68 -68: Property</t>
-  </si>
-  <si>
-    <t>84-84 : Public administration &amp; defence</t>
-  </si>
-  <si>
-    <t>85-85 : Education</t>
+    <t>47 : Retail</t>
+  </si>
+  <si>
+    <t>45 : Motor trades</t>
+  </si>
+  <si>
+    <t>68 : Property</t>
+  </si>
+  <si>
+    <t>84 : Public administration &amp; defence</t>
+  </si>
+  <si>
+    <t>85 : Education</t>
+  </si>
+  <si>
+    <t>46 : Wholesale</t>
   </si>
 </sst>
 </file>
@@ -2781,8 +2781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E1BB99-114C-41D6-9D84-99D5165DE18D}">
   <dimension ref="A1:AM380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2864,13 +2864,13 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>791</v>
+      </c>
+      <c r="O1" t="s">
+        <v>795</v>
+      </c>
+      <c r="P1" t="s">
         <v>790</v>
-      </c>
-      <c r="O1" t="s">
-        <v>792</v>
-      </c>
-      <c r="P1" t="s">
-        <v>791</v>
       </c>
       <c r="Q1" t="s">
         <v>13</v>
@@ -2885,7 +2885,7 @@
         <v>16</v>
       </c>
       <c r="U1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="V1" t="s">
         <v>17</v>
@@ -2894,10 +2894,10 @@
         <v>18</v>
       </c>
       <c r="X1" t="s">
+        <v>793</v>
+      </c>
+      <c r="Y1" t="s">
         <v>794</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>795</v>
       </c>
       <c r="Z1" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Changes in petrol coal and NG consumptions calculations
</commit_message>
<xml_diff>
--- a/ONSData6DistrictLevel.xlsx
+++ b/ONSData6DistrictLevel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fintech Sandpit\ESG-entity-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EA200E-E40D-4A4F-9291-6114A3D63550}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642DEE58-655D-46B8-933D-5E79134625D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{692A125E-7669-4FF7-9E0A-E17AE87AD601}"/>
   </bookViews>
@@ -2781,8 +2781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E1BB99-114C-41D6-9D84-99D5165DE18D}">
   <dimension ref="A1:AM380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>